<commit_message>
change export format. update data. remove unused code. separate save button and delete button
</commit_message>
<xml_diff>
--- a/Archive/ราคาสหกรณ์.xlsx
+++ b/Archive/ราคาสหกรณ์.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fisglobal-my.sharepoint.com/personal/kanyakornploy_kitisopakul_fisglobal_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e1095238\source\repos\myCashier\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{D8A66DF8-847F-43BE-B7F6-27E929DC71EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6909FDE-9B07-4F60-8079-E7D307C10883}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1169133A-B176-4CCB-AF9B-4B5EDCFB2983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ของ!$A$1:$K$568</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="696">
   <si>
     <t>location</t>
   </si>
@@ -2117,10 +2118,16 @@
     <t>ตัด 29/4</t>
   </si>
   <si>
-    <t>พริกแกงญ 40</t>
-  </si>
-  <si>
-    <t>กล้วยทอด 25</t>
+    <t>ปลาทอด 40</t>
+  </si>
+  <si>
+    <t>พริกแกงญ 40 เพิ่ม 20บ มล</t>
+  </si>
+  <si>
+    <t>เปลียนราคากล้วยทอด 25</t>
+  </si>
+  <si>
+    <t>แปรงสีฟัน</t>
   </si>
 </sst>
 </file>
@@ -2143,37 +2150,44 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2248,11 +2262,11 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2473,8 +2487,8 @@
   </sheetPr>
   <dimension ref="A1:N995"/>
   <sheetViews>
-    <sheetView topLeftCell="A549" workbookViewId="0">
-      <selection activeCell="A581" sqref="A581"/>
+    <sheetView topLeftCell="A545" workbookViewId="0">
+      <selection activeCell="K578" sqref="A578:K578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24577,15 +24591,15 @@
         <v>1</v>
       </c>
       <c r="G575" s="3">
-        <f t="shared" ref="G575" si="9">E575/F575</f>
+        <f>E575/F575</f>
         <v>60</v>
       </c>
       <c r="H575" s="3">
-        <f t="shared" ref="H575" si="10">G575*1.15</f>
+        <f>G575*1.15</f>
         <v>69</v>
       </c>
       <c r="I575" s="3">
-        <f t="shared" ref="I575" si="11">D575-G575</f>
+        <f>D575-G575</f>
         <v>5</v>
       </c>
       <c r="J575">
@@ -24615,15 +24629,15 @@
         <v>1</v>
       </c>
       <c r="G576" s="3">
-        <f t="shared" ref="G576:G577" si="12">E576/F576</f>
+        <f>E576/F576</f>
         <v>40</v>
       </c>
       <c r="H576" s="3">
-        <f t="shared" ref="H576:H577" si="13">G576*1.15</f>
+        <f>G576*1.15</f>
         <v>46</v>
       </c>
       <c r="I576" s="3">
-        <f t="shared" ref="I576:I577" si="14">D576-G576</f>
+        <f>D576-G576</f>
         <v>5</v>
       </c>
       <c r="J576">
@@ -24653,26 +24667,61 @@
         <v>6</v>
       </c>
       <c r="G577" s="3">
-        <f t="shared" si="12"/>
+        <f>E577/F577</f>
         <v>8.25</v>
       </c>
       <c r="H577" s="3">
-        <f t="shared" si="13"/>
+        <f>G577*1.15</f>
         <v>9.4874999999999989</v>
       </c>
       <c r="I577" s="3">
-        <f t="shared" si="14"/>
+        <f>D577-G577</f>
         <v>1.75</v>
       </c>
       <c r="J577" s="4">
         <v>0</v>
       </c>
-      <c r="K577" s="27" t="s">
+      <c r="K577" s="25" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="578" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K578" s="11"/>
+    <row r="578" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A578" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B578" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C578" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="D578" s="3">
+        <v>40</v>
+      </c>
+      <c r="E578" s="3">
+        <v>35</v>
+      </c>
+      <c r="F578" s="3">
+        <v>1</v>
+      </c>
+      <c r="G578" s="3">
+        <f>E578/F578</f>
+        <v>35</v>
+      </c>
+      <c r="H578" s="3">
+        <f>G578*1.15</f>
+        <v>40.25</v>
+      </c>
+      <c r="I578" s="3">
+        <f>D578-G578</f>
+        <v>5</v>
+      </c>
+      <c r="J578" s="4">
+        <v>0</v>
+      </c>
+      <c r="K578" s="7" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="579" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K579" s="11"/>
@@ -26085,10 +26134,10 @@
       <c r="E15" s="20" t="s">
         <v>626</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="26" t="s">
         <v>627</v>
       </c>
-      <c r="G15" s="26"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
@@ -26282,20 +26331,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:C29"/>
+  <dimension ref="A2:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>644</v>
       </c>
@@ -26303,7 +26352,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>646</v>
       </c>
@@ -26311,12 +26360,12 @@
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>649</v>
       </c>
@@ -26324,7 +26373,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>644</v>
       </c>
@@ -26332,7 +26381,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>644</v>
       </c>
@@ -26340,7 +26389,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>633</v>
       </c>
@@ -26351,7 +26400,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>644</v>
       </c>
@@ -26359,7 +26408,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>644</v>
       </c>
@@ -26370,7 +26419,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>633</v>
       </c>
@@ -26381,7 +26430,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>633</v>
       </c>
@@ -26392,7 +26441,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>633</v>
       </c>
@@ -26400,7 +26449,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>633</v>
       </c>
@@ -26408,7 +26457,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>633</v>
       </c>
@@ -26416,42 +26465,42 @@
         <v>661</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="14" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>633</v>
       </c>
@@ -26459,7 +26508,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>633</v>
       </c>
@@ -26474,12 +26523,17 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="14" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="14" t="s">
-        <v>693</v>
+        <v>694</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="14" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>